<commit_message>
buff aug a3 folded foregrip
</commit_message>
<xml_diff>
--- a/changes/foregrips.xlsx
+++ b/changes/foregrips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B023C743-3C68-4849-BFD6-D451CA2E3A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0981D8E7-4C3A-4EB5-9F0B-8550938661FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foregrips" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>magazine_capacity</t>
   </si>
   <si>
-    <t>bullet_deviation</t>
-  </si>
-  <si>
     <t>bullet_damage</t>
   </si>
   <si>
@@ -450,6 +447,9 @@
   </si>
   <si>
     <t>magpul_mvg_mag597_foregrip</t>
+  </si>
+  <si>
+    <t>barrel_deviation</t>
   </si>
 </sst>
 </file>
@@ -1316,21 +1316,21 @@
   <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1353,45 +1353,45 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
       <c r="P2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>122</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>123</v>
       </c>
-      <c r="S2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>105</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>106</v>
       </c>
       <c r="C3" s="21">
         <v>6</v>
@@ -1419,12 +1419,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>107</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>108</v>
       </c>
       <c r="C4" s="22">
         <v>4</v>
@@ -1452,12 +1452,12 @@
         <v>6.9999999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="23">
         <v>4</v>
@@ -1485,12 +1485,12 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>109</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>110</v>
       </c>
       <c r="C6" s="23">
         <v>1</v>
@@ -1518,12 +1518,12 @@
         <v>5.1999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>111</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>112</v>
       </c>
       <c r="C7" s="23">
         <v>4</v>
@@ -1551,12 +1551,12 @@
         <v>5.7999999999999989</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>114</v>
       </c>
       <c r="C8" s="23">
         <v>4</v>
@@ -1584,12 +1584,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>115</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>116</v>
       </c>
       <c r="C9" s="23">
         <v>6</v>
@@ -1617,12 +1617,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1644,12 +1644,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1671,12 +1671,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -1698,12 +1698,12 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -1725,12 +1725,12 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>117</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>118</v>
       </c>
       <c r="C14" s="23">
         <v>4</v>
@@ -1752,12 +1752,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>133</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>134</v>
       </c>
       <c r="C15" s="23">
         <v>6</v>
@@ -1779,18 +1779,18 @@
         <v>6.1999999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N16" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -1818,12 +1818,12 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>85</v>
       </c>
       <c r="C18" s="18">
         <v>-1</v>
@@ -1851,12 +1851,12 @@
         <v>3.4000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="18">
         <v>-3</v>
@@ -1884,12 +1884,12 @@
         <v>4.2000000000000011</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="C20" s="17">
         <v>0</v>
@@ -1917,12 +1917,12 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C21" s="17">
         <v>-1</v>
@@ -1950,12 +1950,12 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="C22" s="17">
         <v>-3</v>
@@ -1983,12 +1983,12 @@
         <v>3.3999999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
@@ -2016,12 +2016,12 @@
         <v>3.9999999999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>129</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>130</v>
       </c>
       <c r="C24" s="23">
         <v>6</v>
@@ -2043,12 +2043,12 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -2076,12 +2076,12 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C26" s="7">
         <v>6</v>
@@ -2109,12 +2109,12 @@
         <v>7.0000000000000009</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
@@ -2142,12 +2142,12 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C28" s="5">
         <v>2</v>
@@ -2175,12 +2175,12 @@
         <v>6.8000000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C29" s="6">
         <v>4</v>
@@ -2208,12 +2208,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="C30" s="7">
         <v>4</v>
@@ -2241,12 +2241,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="C31" s="8">
         <v>3</v>
@@ -2274,12 +2274,12 @@
         <v>7.0000000000000009</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -2307,12 +2307,12 @@
         <v>5.1999999999999993</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="C33" s="9">
         <v>4</v>
@@ -2340,12 +2340,12 @@
         <v>5.7999999999999989</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="C34" s="10">
         <v>3</v>
@@ -2373,12 +2373,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="C35" s="12">
         <v>4</v>
@@ -2406,12 +2406,12 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="C36" s="13">
         <v>2</v>
@@ -2439,12 +2439,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="C37" s="14">
         <v>3</v>
@@ -2472,12 +2472,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>66</v>
       </c>
       <c r="C38" s="23">
         <v>3</v>
@@ -2505,12 +2505,12 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="23">
         <v>6</v>
@@ -2538,12 +2538,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="C40" s="15">
         <v>4</v>
@@ -2571,12 +2571,12 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="C41" s="15">
         <v>5</v>
@@ -2604,12 +2604,12 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="C42" s="16">
         <v>5</v>
@@ -2637,12 +2637,12 @@
         <v>7.2000000000000011</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="C43" s="17">
         <v>5</v>
@@ -2670,12 +2670,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" t="s">
-        <v>24</v>
       </c>
       <c r="C44">
         <v>5</v>
@@ -2697,12 +2697,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
         <v>25</v>
-      </c>
-      <c r="B45" t="s">
-        <v>26</v>
       </c>
       <c r="C45" s="23">
         <v>5</v>
@@ -2724,12 +2724,12 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" t="s">
         <v>27</v>
-      </c>
-      <c r="B46" t="s">
-        <v>28</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -2751,12 +2751,12 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
         <v>29</v>
-      </c>
-      <c r="B47" t="s">
-        <v>30</v>
       </c>
       <c r="C47" s="23">
         <v>6</v>
@@ -2778,12 +2778,12 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>120</v>
       </c>
       <c r="C48" s="23">
         <v>4</v>
@@ -2819,18 +2819,18 @@
         <v>8.199999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N49" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="C50" s="11">
         <v>-1</v>
@@ -2858,12 +2858,12 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="C51" s="11">
         <v>-0.5</v>
@@ -2891,12 +2891,12 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="C52" s="11">
         <v>-0.5</v>
@@ -2924,12 +2924,12 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>87</v>
       </c>
       <c r="C53" s="19">
         <v>3</v>
@@ -2957,12 +2957,12 @@
         <v>7.8000000000000007</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>88</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>89</v>
       </c>
       <c r="C54" s="19">
         <v>1</v>
@@ -2990,12 +2990,12 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="C55" s="19">
         <v>-1</v>
@@ -3023,12 +3023,12 @@
         <v>6.3999999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="C56" s="19">
         <v>4</v>
@@ -3056,12 +3056,12 @@
         <v>7.8000000000000007</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="C57" s="19">
         <v>3</v>
@@ -3089,12 +3089,12 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="C58" s="19">
         <v>5</v>
@@ -3122,12 +3122,12 @@
         <v>7.6000000000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C59" s="20">
         <v>3</v>
@@ -3155,12 +3155,12 @@
         <v>7.8000000000000007</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="20">
         <v>1</v>
@@ -3188,12 +3188,12 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="20">
         <v>-1</v>
@@ -3221,12 +3221,12 @@
         <v>6.3999999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C62" s="20">
         <v>4</v>
@@ -3254,12 +3254,12 @@
         <v>7.8000000000000007</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="B63" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="C63" s="20">
         <v>3</v>
@@ -3287,12 +3287,12 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" s="20">
         <v>5</v>
@@ -3320,18 +3320,18 @@
         <v>7.6000000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N65" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" s="23" t="s">
         <v>125</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>126</v>
       </c>
       <c r="C66" s="23">
         <v>2</v>
@@ -3359,12 +3359,12 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="23" t="s">
         <v>127</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>128</v>
       </c>
       <c r="C67" s="23">
         <v>7</v>
@@ -3373,14 +3373,14 @@
         <v>0.1</v>
       </c>
       <c r="E67" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" s="23">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G67" s="23"/>
       <c r="H67" s="23">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I67" s="23"/>
       <c r="J67" s="23"/>
@@ -3390,22 +3390,22 @@
         <v>0</v>
       </c>
       <c r="N67" s="23">
-        <f t="shared" si="0"/>
-        <v>3.1999999999999997</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+        <f>C67-D67*20-E67*0.8-F67*0.6-H67*2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N68" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" t="s">
         <v>131</v>
-      </c>
-      <c r="B69" t="s">
-        <v>132</v>
       </c>
       <c r="C69">
         <v>3</v>

</xml_diff>